<commit_message>
Add KEGG_Pathways as primary source.
</commit_message>
<xml_diff>
--- a/data/Resource Interaction Table-withIntegrated.xlsx
+++ b/data/Resource Interaction Table-withIntegrated.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brooksantangelo/Documents/ReviewPaper/db_review/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7474F1-5770-DF46-B964-1541D1A1E3BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541358C0-3B40-F941-9074-92C0160DED51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-1780" windowWidth="33480" windowHeight="18720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25920" yWindow="500" windowWidth="25920" windowHeight="17680" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1454" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1462" uniqueCount="79">
   <si>
     <t>source</t>
   </si>
@@ -257,6 +257,9 @@
   </si>
   <si>
     <t>has nomenclature mapping</t>
+  </si>
+  <si>
+    <t>KEGG_Pathways</t>
   </si>
 </sst>
 </file>
@@ -527,10 +530,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D148"/>
+  <dimension ref="A1:D149"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1267,13 +1270,13 @@
     </row>
     <row r="67" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A67" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>5</v>
+        <v>78</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1284,7 +1287,7 @@
         <v>76</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1295,18 +1298,18 @@
         <v>76</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A70" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>76</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1314,10 +1317,10 @@
         <v>34</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1325,10 +1328,10 @@
         <v>34</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1336,10 +1339,10 @@
         <v>34</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1350,7 +1353,7 @@
         <v>77</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1361,7 +1364,7 @@
         <v>77</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1372,7 +1375,7 @@
         <v>77</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1383,7 +1386,7 @@
         <v>77</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1391,10 +1394,10 @@
         <v>34</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1402,10 +1405,10 @@
         <v>34</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1416,18 +1419,18 @@
         <v>77</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A81" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>77</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -1438,7 +1441,7 @@
         <v>77</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="D82" s="1"/>
     </row>
@@ -1461,7 +1464,7 @@
         <v>77</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -1472,18 +1475,18 @@
         <v>77</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A86" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -1491,10 +1494,10 @@
         <v>37</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -1505,18 +1508,18 @@
         <v>77</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A89" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -1524,10 +1527,10 @@
         <v>38</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>74</v>
+        <v>33</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -1538,7 +1541,7 @@
         <v>77</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -1549,29 +1552,29 @@
         <v>77</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A93" s="2" t="s">
+      <c r="A93" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="B93" s="1" t="s">
         <v>77</v>
       </c>
       <c r="C93" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="13" x14ac:dyDescent="0.15">
+      <c r="A94" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C94" s="1" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A94" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -1582,7 +1585,7 @@
         <v>77</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -1590,10 +1593,10 @@
         <v>38</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1604,7 +1607,7 @@
         <v>76</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1612,21 +1615,21 @@
         <v>38</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A99" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1634,21 +1637,21 @@
         <v>41</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A101" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1656,21 +1659,21 @@
         <v>42</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A103" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>77</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1681,7 +1684,7 @@
         <v>77</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1692,7 +1695,7 @@
         <v>77</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1700,15 +1703,15 @@
         <v>44</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A107" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>76</v>
@@ -1722,10 +1725,10 @@
         <v>46</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1736,7 +1739,7 @@
         <v>77</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1747,7 +1750,7 @@
         <v>77</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1758,7 +1761,7 @@
         <v>77</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1769,7 +1772,7 @@
         <v>77</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1780,18 +1783,18 @@
         <v>77</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A114" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C114" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1802,7 +1805,7 @@
         <v>76</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1810,10 +1813,10 @@
         <v>47</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1824,7 +1827,7 @@
         <v>77</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1835,7 +1838,7 @@
         <v>77</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1846,7 +1849,7 @@
         <v>77</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1857,7 +1860,7 @@
         <v>77</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1865,10 +1868,10 @@
         <v>47</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1876,21 +1879,21 @@
         <v>47</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A123" s="1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1901,7 +1904,7 @@
         <v>76</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1909,21 +1912,21 @@
         <v>40</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A126" s="1" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1934,7 +1937,7 @@
         <v>76</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1942,10 +1945,10 @@
         <v>55</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1956,18 +1959,18 @@
         <v>77</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A130" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>77</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1978,7 +1981,7 @@
         <v>77</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1989,7 +1992,7 @@
         <v>77</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2000,7 +2003,7 @@
         <v>77</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2011,7 +2014,7 @@
         <v>77</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2022,18 +2025,18 @@
         <v>77</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A136" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>77</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2044,7 +2047,7 @@
         <v>77</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2052,21 +2055,21 @@
         <v>57</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="139" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A139" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2074,26 +2077,26 @@
         <v>64</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C140" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A141" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C141" s="1" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A141" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B141" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C141" s="2" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A142" s="2" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>76</v>
@@ -2104,7 +2107,7 @@
     </row>
     <row r="143" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A143" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>76</v>
@@ -2115,13 +2118,13 @@
     </row>
     <row r="144" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A144" s="2" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>76</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>5</v>
+        <v>66</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2129,10 +2132,10 @@
         <v>70</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2143,7 +2146,7 @@
         <v>77</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="147" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2154,17 +2157,28 @@
         <v>77</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="148" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A148" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A149" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B148" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C148" s="2" t="s">
+      <c r="B149" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C149" s="2" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2179,10 +2193,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B61"/>
+  <dimension ref="A1:B62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2679,6 +2693,14 @@
         <v>68</v>
       </c>
     </row>
+    <row r="62" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A62" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2688,8 +2710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C62B794-0898-E64A-A668-9B45516A9588}">
   <dimension ref="A1:C148"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="A76" sqref="A1:C1048576"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C153" sqref="C153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4333,10 +4355,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C62C224-E054-A841-B649-DAD5203F257C}">
-  <dimension ref="A1:C148"/>
+  <dimension ref="A1:C149"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="109" workbookViewId="0">
+      <selection activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5073,13 +5095,13 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A67" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>5</v>
+        <v>78</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.15">
@@ -5087,10 +5109,10 @@
         <v>32</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.15">
@@ -5098,21 +5120,21 @@
         <v>32</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A70" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.15">
@@ -5123,7 +5145,7 @@
         <v>4</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.15">
@@ -5131,10 +5153,10 @@
         <v>34</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.15">
@@ -5145,7 +5167,7 @@
         <v>6</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.15">
@@ -5156,7 +5178,7 @@
         <v>6</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.15">
@@ -5167,7 +5189,7 @@
         <v>6</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.15">
@@ -5178,7 +5200,7 @@
         <v>6</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.15">
@@ -5189,7 +5211,7 @@
         <v>6</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.15">
@@ -5197,10 +5219,10 @@
         <v>34</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.15">
@@ -5211,7 +5233,7 @@
         <v>14</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.15">
@@ -5222,18 +5244,18 @@
         <v>14</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A81" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.15">
@@ -5241,10 +5263,10 @@
         <v>35</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.15">
@@ -5252,7 +5274,7 @@
         <v>35</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>28</v>
@@ -5263,10 +5285,10 @@
         <v>35</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.15">
@@ -5274,21 +5296,21 @@
         <v>35</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A86" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.15">
@@ -5299,7 +5321,7 @@
         <v>6</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.15">
@@ -5307,21 +5329,21 @@
         <v>37</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A89" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.15">
@@ -5332,7 +5354,7 @@
         <v>10</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>74</v>
+        <v>33</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.15">
@@ -5343,7 +5365,7 @@
         <v>10</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.15">
@@ -5354,29 +5376,29 @@
         <v>10</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A93" s="2" t="s">
+      <c r="A93" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="B93" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C93" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A94" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C94" s="1" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A94" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.15">
@@ -5387,7 +5409,7 @@
         <v>6</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.15">
@@ -5395,10 +5417,10 @@
         <v>38</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.15">
@@ -5406,10 +5428,10 @@
         <v>38</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.15">
@@ -5417,21 +5439,21 @@
         <v>38</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A99" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.15">
@@ -5439,21 +5461,21 @@
         <v>41</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A101" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.15">
@@ -5461,21 +5483,21 @@
         <v>42</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A103" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.15">
@@ -5483,10 +5505,10 @@
         <v>44</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.15">
@@ -5497,7 +5519,7 @@
         <v>10</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.15">
@@ -5505,15 +5527,15 @@
         <v>44</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A107" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>4</v>
@@ -5527,10 +5549,10 @@
         <v>46</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.15">
@@ -5541,7 +5563,7 @@
         <v>6</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.15">
@@ -5552,7 +5574,7 @@
         <v>6</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.15">
@@ -5560,10 +5582,10 @@
         <v>46</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.15">
@@ -5574,7 +5596,7 @@
         <v>10</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.15">
@@ -5585,18 +5607,18 @@
         <v>10</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A114" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C114" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.15">
@@ -5604,10 +5626,10 @@
         <v>47</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.15">
@@ -5618,7 +5640,7 @@
         <v>6</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.15">
@@ -5629,7 +5651,7 @@
         <v>6</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.15">
@@ -5640,7 +5662,7 @@
         <v>6</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.15">
@@ -5651,7 +5673,7 @@
         <v>6</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.15">
@@ -5659,10 +5681,10 @@
         <v>47</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.15">
@@ -5673,7 +5695,7 @@
         <v>10</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.15">
@@ -5684,18 +5706,18 @@
         <v>10</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A123" s="1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.15">
@@ -5703,10 +5725,10 @@
         <v>40</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.15">
@@ -5717,18 +5739,18 @@
         <v>10</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A126" s="1" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.15">
@@ -5736,10 +5758,10 @@
         <v>55</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.15">
@@ -5750,7 +5772,7 @@
         <v>14</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.15">
@@ -5761,18 +5783,18 @@
         <v>14</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A130" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.15">
@@ -5783,7 +5805,7 @@
         <v>14</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.15">
@@ -5794,7 +5816,7 @@
         <v>14</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.15">
@@ -5802,10 +5824,10 @@
         <v>56</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.15">
@@ -5816,7 +5838,7 @@
         <v>4</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.15">
@@ -5827,18 +5849,18 @@
         <v>4</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A136" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.15">
@@ -5849,7 +5871,7 @@
         <v>4</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.15">
@@ -5857,21 +5879,21 @@
         <v>57</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A139" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.15">
@@ -5879,26 +5901,26 @@
         <v>64</v>
       </c>
       <c r="B140" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A141" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B141" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C140" s="1" t="s">
+      <c r="C141" s="1" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A141" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B141" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C141" s="2" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A142" s="2" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B142" s="2" t="s">
         <v>36</v>
@@ -5909,7 +5931,7 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A143" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B143" s="2" t="s">
         <v>36</v>
@@ -5920,13 +5942,13 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A144" s="2" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>5</v>
+        <v>66</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.15">
@@ -5937,7 +5959,7 @@
         <v>4</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.15">
@@ -5945,10 +5967,10 @@
         <v>70</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.15">
@@ -5959,17 +5981,28 @@
         <v>10</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A148" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A149" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B148" s="2" t="s">
+      <c r="B149" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C148" s="2" t="s">
+      <c r="C149" s="2" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Replace snomed with snomed ct.
</commit_message>
<xml_diff>
--- a/data/Resource Interaction Table-withIntegrated.xlsx
+++ b/data/Resource Interaction Table-withIntegrated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brooksantangelo/Documents/ReviewPaper/db_review/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541358C0-3B40-F941-9074-92C0160DED51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8399D2C-2E5D-2D41-88E3-00920F930A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25920" yWindow="500" windowWidth="25920" windowHeight="17680" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -208,12 +208,6 @@
     <t>UMLS_Microbe</t>
   </si>
   <si>
-    <t>SNOMED_Microbe</t>
-  </si>
-  <si>
-    <t>SNOMED_Disease</t>
-  </si>
-  <si>
     <t>UMLS_Disease</t>
   </si>
   <si>
@@ -260,6 +254,12 @@
   </si>
   <si>
     <t>KEGG_Pathways</t>
+  </si>
+  <si>
+    <t>SNOMEDCT_Microbe</t>
+  </si>
+  <si>
+    <t>SNOMEDCT_Disease</t>
   </si>
 </sst>
 </file>
@@ -532,8 +532,8 @@
   </sheetPr>
   <dimension ref="A1:D149"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="E130" sqref="E130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -558,7 +558,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
@@ -569,7 +569,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -580,7 +580,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>8</v>
@@ -591,7 +591,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>9</v>
@@ -602,7 +602,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>11</v>
@@ -613,7 +613,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>5</v>
@@ -624,7 +624,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>13</v>
@@ -635,7 +635,7 @@
         <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>15</v>
@@ -646,7 +646,7 @@
         <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>5</v>
@@ -657,7 +657,7 @@
         <v>16</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>17</v>
@@ -668,7 +668,7 @@
         <v>16</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>18</v>
@@ -679,7 +679,7 @@
         <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>13</v>
@@ -690,7 +690,7 @@
         <v>19</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>20</v>
@@ -701,7 +701,7 @@
         <v>9</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>21</v>
@@ -712,7 +712,7 @@
         <v>9</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>7</v>
@@ -723,7 +723,7 @@
         <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>8</v>
@@ -734,7 +734,7 @@
         <v>9</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>20</v>
@@ -745,7 +745,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>22</v>
@@ -756,7 +756,7 @@
         <v>9</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>23</v>
@@ -767,10 +767,10 @@
         <v>9</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -778,10 +778,10 @@
         <v>9</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -789,7 +789,7 @@
         <v>24</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>25</v>
@@ -800,7 +800,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>7</v>
@@ -811,7 +811,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>8</v>
@@ -822,7 +822,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>26</v>
@@ -833,7 +833,7 @@
         <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>11</v>
@@ -844,7 +844,7 @@
         <v>24</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>20</v>
@@ -855,7 +855,7 @@
         <v>24</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>22</v>
@@ -866,7 +866,7 @@
         <v>24</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>9</v>
@@ -877,7 +877,7 @@
         <v>27</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>7</v>
@@ -888,7 +888,7 @@
         <v>27</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>8</v>
@@ -899,7 +899,7 @@
         <v>27</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>26</v>
@@ -910,7 +910,7 @@
         <v>27</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>20</v>
@@ -921,7 +921,7 @@
         <v>27</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>9</v>
@@ -932,7 +932,7 @@
         <v>27</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>24</v>
@@ -943,7 +943,7 @@
         <v>27</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>28</v>
@@ -954,7 +954,7 @@
         <v>29</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>7</v>
@@ -965,7 +965,7 @@
         <v>29</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>8</v>
@@ -976,7 +976,7 @@
         <v>29</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>13</v>
@@ -987,7 +987,7 @@
         <v>29</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>26</v>
@@ -998,7 +998,7 @@
         <v>29</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>11</v>
@@ -1009,7 +1009,7 @@
         <v>29</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>20</v>
@@ -1020,7 +1020,7 @@
         <v>29</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>23</v>
@@ -1031,7 +1031,7 @@
         <v>29</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>24</v>
@@ -1042,7 +1042,7 @@
         <v>29</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>30</v>
@@ -1053,7 +1053,7 @@
         <v>29</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>9</v>
@@ -1064,7 +1064,7 @@
         <v>29</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>28</v>
@@ -1075,7 +1075,7 @@
         <v>30</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>7</v>
@@ -1086,7 +1086,7 @@
         <v>30</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>26</v>
@@ -1097,7 +1097,7 @@
         <v>30</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>28</v>
@@ -1108,7 +1108,7 @@
         <v>30</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>24</v>
@@ -1119,7 +1119,7 @@
         <v>31</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>5</v>
@@ -1130,7 +1130,7 @@
         <v>31</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>7</v>
@@ -1141,7 +1141,7 @@
         <v>31</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>26</v>
@@ -1152,7 +1152,7 @@
         <v>31</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>20</v>
@@ -1163,7 +1163,7 @@
         <v>31</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>30</v>
@@ -1174,7 +1174,7 @@
         <v>31</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>28</v>
@@ -1185,7 +1185,7 @@
         <v>28</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>21</v>
@@ -1196,7 +1196,7 @@
         <v>28</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>25</v>
@@ -1207,7 +1207,7 @@
         <v>28</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>5</v>
@@ -1218,7 +1218,7 @@
         <v>28</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>7</v>
@@ -1229,7 +1229,7 @@
         <v>28</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>8</v>
@@ -1240,7 +1240,7 @@
         <v>28</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>11</v>
@@ -1251,7 +1251,7 @@
         <v>28</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>20</v>
@@ -1262,7 +1262,7 @@
         <v>28</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>58</v>
@@ -1273,10 +1273,10 @@
         <v>28</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1284,7 +1284,7 @@
         <v>32</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>5</v>
@@ -1295,7 +1295,7 @@
         <v>32</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>7</v>
@@ -1306,7 +1306,7 @@
         <v>32</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>33</v>
@@ -1317,7 +1317,7 @@
         <v>34</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>5</v>
@@ -1328,7 +1328,7 @@
         <v>34</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>21</v>
@@ -1339,7 +1339,7 @@
         <v>34</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>7</v>
@@ -1350,7 +1350,7 @@
         <v>34</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>28</v>
@@ -1361,7 +1361,7 @@
         <v>34</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>29</v>
@@ -1372,7 +1372,7 @@
         <v>34</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>26</v>
@@ -1383,7 +1383,7 @@
         <v>34</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>8</v>
@@ -1394,7 +1394,7 @@
         <v>34</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>9</v>
@@ -1405,7 +1405,7 @@
         <v>34</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>15</v>
@@ -1416,10 +1416,10 @@
         <v>34</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -1427,7 +1427,7 @@
         <v>34</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>45</v>
@@ -1438,7 +1438,7 @@
         <v>35</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>58</v>
@@ -1450,7 +1450,7 @@
         <v>35</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>28</v>
@@ -1461,10 +1461,10 @@
         <v>35</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -1472,7 +1472,7 @@
         <v>35</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>59</v>
@@ -1483,7 +1483,7 @@
         <v>35</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>58</v>
@@ -1494,7 +1494,7 @@
         <v>37</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>7</v>
@@ -1505,7 +1505,7 @@
         <v>37</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>9</v>
@@ -1516,7 +1516,7 @@
         <v>37</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>11</v>
@@ -1527,7 +1527,7 @@
         <v>38</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>33</v>
@@ -1538,10 +1538,10 @@
         <v>38</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -1549,10 +1549,10 @@
         <v>38</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -1560,7 +1560,7 @@
         <v>38</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>28</v>
@@ -1571,7 +1571,7 @@
         <v>38</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>20</v>
@@ -1582,7 +1582,7 @@
         <v>38</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>26</v>
@@ -1593,7 +1593,7 @@
         <v>38</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>39</v>
@@ -1604,7 +1604,7 @@
         <v>38</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>15</v>
@@ -1615,7 +1615,7 @@
         <v>38</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>7</v>
@@ -1626,7 +1626,7 @@
         <v>38</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>40</v>
@@ -1637,7 +1637,7 @@
         <v>41</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>5</v>
@@ -1648,7 +1648,7 @@
         <v>41</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>11</v>
@@ -1659,7 +1659,7 @@
         <v>42</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>5</v>
@@ -1670,7 +1670,7 @@
         <v>42</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>43</v>
@@ -1681,7 +1681,7 @@
         <v>44</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>45</v>
@@ -1692,7 +1692,7 @@
         <v>44</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>20</v>
@@ -1703,7 +1703,7 @@
         <v>44</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>28</v>
@@ -1714,7 +1714,7 @@
         <v>44</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>5</v>
@@ -1725,7 +1725,7 @@
         <v>46</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>5</v>
@@ -1736,7 +1736,7 @@
         <v>46</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>28</v>
@@ -1747,7 +1747,7 @@
         <v>46</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>24</v>
@@ -1758,7 +1758,7 @@
         <v>46</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>47</v>
@@ -1769,7 +1769,7 @@
         <v>46</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>28</v>
@@ -1780,7 +1780,7 @@
         <v>46</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>24</v>
@@ -1791,7 +1791,7 @@
         <v>46</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>47</v>
@@ -1802,7 +1802,7 @@
         <v>47</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>5</v>
@@ -1813,7 +1813,7 @@
         <v>47</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>7</v>
@@ -1824,7 +1824,7 @@
         <v>47</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>24</v>
@@ -1835,7 +1835,7 @@
         <v>47</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>38</v>
@@ -1846,7 +1846,7 @@
         <v>47</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>9</v>
@@ -1857,7 +1857,7 @@
         <v>47</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>28</v>
@@ -1868,7 +1868,7 @@
         <v>47</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>20</v>
@@ -1879,7 +1879,7 @@
         <v>47</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>33</v>
@@ -1890,7 +1890,7 @@
         <v>47</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>48</v>
@@ -1901,7 +1901,7 @@
         <v>40</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>5</v>
@@ -1912,7 +1912,7 @@
         <v>40</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>33</v>
@@ -1923,7 +1923,7 @@
         <v>40</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>38</v>
@@ -1934,7 +1934,7 @@
         <v>55</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>5</v>
@@ -1945,7 +1945,7 @@
         <v>55</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>15</v>
@@ -1956,10 +1956,10 @@
         <v>55</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1967,7 +1967,7 @@
         <v>55</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>45</v>
@@ -1978,10 +1978,10 @@
         <v>56</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1989,7 +1989,7 @@
         <v>56</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>58</v>
@@ -2000,10 +2000,10 @@
         <v>56</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2011,7 +2011,7 @@
         <v>56</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>59</v>
@@ -2022,10 +2022,10 @@
         <v>56</v>
       </c>
       <c r="B135" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C135" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="C135" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2033,7 +2033,7 @@
         <v>56</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>60</v>
@@ -2044,7 +2044,7 @@
         <v>57</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>17</v>
@@ -2055,7 +2055,7 @@
         <v>57</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>5</v>
@@ -2066,7 +2066,7 @@
         <v>57</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C139" s="1" t="s">
         <v>15</v>
@@ -2074,10 +2074,10 @@
     </row>
     <row r="140" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A140" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>5</v>
@@ -2085,13 +2085,13 @@
     </row>
     <row r="141" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A141" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2099,10 +2099,10 @@
         <v>24</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2110,10 +2110,10 @@
         <v>37</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2121,18 +2121,18 @@
         <v>38</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A145" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C145" s="2" t="s">
         <v>5</v>
@@ -2140,10 +2140,10 @@
     </row>
     <row r="146" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A146" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C146" s="2" t="s">
         <v>21</v>
@@ -2151,10 +2151,10 @@
     </row>
     <row r="147" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A147" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C147" s="2" t="s">
         <v>22</v>
@@ -2162,10 +2162,10 @@
     </row>
     <row r="148" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A148" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C148" s="2" t="s">
         <v>20</v>
@@ -2173,10 +2173,10 @@
     </row>
     <row r="149" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A149" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C149" s="2" t="s">
         <v>28</v>
@@ -2196,7 +2196,7 @@
   <dimension ref="A1:B62"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2338,7 +2338,7 @@
         <v>28</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2346,7 +2346,7 @@
         <v>24</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2354,7 +2354,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2362,7 +2362,7 @@
         <v>30</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2370,7 +2370,7 @@
         <v>29</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2394,7 +2394,7 @@
         <v>47</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2402,7 +2402,7 @@
         <v>38</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2418,7 +2418,7 @@
         <v>3</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2426,7 +2426,7 @@
         <v>12</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2434,7 +2434,7 @@
         <v>16</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2442,7 +2442,7 @@
         <v>19</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2450,7 +2450,7 @@
         <v>27</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2458,7 +2458,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2466,7 +2466,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2474,7 +2474,7 @@
         <v>34</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2482,7 +2482,7 @@
         <v>35</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2490,7 +2490,7 @@
         <v>37</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2498,7 +2498,7 @@
         <v>41</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2506,7 +2506,7 @@
         <v>42</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2522,7 +2522,7 @@
         <v>40</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2530,7 +2530,7 @@
         <v>44</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2538,7 +2538,7 @@
         <v>46</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2546,7 +2546,7 @@
         <v>55</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2554,7 +2554,7 @@
         <v>56</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2562,7 +2562,7 @@
         <v>57</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2575,7 +2575,7 @@
     </row>
     <row r="47" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>54</v>
@@ -2583,7 +2583,7 @@
     </row>
     <row r="48" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>54</v>
@@ -2599,7 +2599,7 @@
     </row>
     <row r="50" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="2" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>51</v>
@@ -2615,23 +2615,23 @@
     </row>
     <row r="52" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>54</v>
@@ -2671,34 +2671,34 @@
     </row>
     <row r="59" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -2710,8 +2710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C62B794-0898-E64A-A668-9B45516A9588}">
   <dimension ref="A1:C148"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C153" sqref="C153"/>
+    <sheetView topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="C134" sqref="C134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2736,7 +2736,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
@@ -2747,7 +2747,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -2758,7 +2758,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>8</v>
@@ -2769,7 +2769,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>9</v>
@@ -2780,7 +2780,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>11</v>
@@ -2791,7 +2791,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>5</v>
@@ -2802,7 +2802,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>13</v>
@@ -2813,7 +2813,7 @@
         <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>15</v>
@@ -2824,7 +2824,7 @@
         <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>5</v>
@@ -2835,7 +2835,7 @@
         <v>16</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>17</v>
@@ -2846,7 +2846,7 @@
         <v>16</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>18</v>
@@ -2857,7 +2857,7 @@
         <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>13</v>
@@ -2868,7 +2868,7 @@
         <v>19</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>20</v>
@@ -2879,7 +2879,7 @@
         <v>9</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>21</v>
@@ -2890,7 +2890,7 @@
         <v>9</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>7</v>
@@ -2901,7 +2901,7 @@
         <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>8</v>
@@ -2912,7 +2912,7 @@
         <v>9</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>20</v>
@@ -2923,7 +2923,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>22</v>
@@ -2934,7 +2934,7 @@
         <v>9</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>23</v>
@@ -2945,10 +2945,10 @@
         <v>9</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
@@ -2956,10 +2956,10 @@
         <v>9</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
@@ -2967,7 +2967,7 @@
         <v>24</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>25</v>
@@ -2978,7 +2978,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>7</v>
@@ -2989,7 +2989,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>8</v>
@@ -3000,7 +3000,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>26</v>
@@ -3011,7 +3011,7 @@
         <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>11</v>
@@ -3022,7 +3022,7 @@
         <v>24</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>20</v>
@@ -3033,7 +3033,7 @@
         <v>24</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>22</v>
@@ -3044,7 +3044,7 @@
         <v>24</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>9</v>
@@ -3055,7 +3055,7 @@
         <v>27</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>7</v>
@@ -3066,7 +3066,7 @@
         <v>27</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>8</v>
@@ -3077,7 +3077,7 @@
         <v>27</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>26</v>
@@ -3088,7 +3088,7 @@
         <v>27</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>20</v>
@@ -3099,7 +3099,7 @@
         <v>27</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>9</v>
@@ -3110,7 +3110,7 @@
         <v>27</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>24</v>
@@ -3121,7 +3121,7 @@
         <v>27</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>28</v>
@@ -3132,7 +3132,7 @@
         <v>29</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>7</v>
@@ -3143,7 +3143,7 @@
         <v>29</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>8</v>
@@ -3154,7 +3154,7 @@
         <v>29</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>13</v>
@@ -3165,7 +3165,7 @@
         <v>29</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>26</v>
@@ -3176,7 +3176,7 @@
         <v>29</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>11</v>
@@ -3187,7 +3187,7 @@
         <v>29</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>20</v>
@@ -3198,7 +3198,7 @@
         <v>29</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>23</v>
@@ -3209,7 +3209,7 @@
         <v>29</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>24</v>
@@ -3220,7 +3220,7 @@
         <v>29</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>30</v>
@@ -3231,7 +3231,7 @@
         <v>29</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>9</v>
@@ -3242,7 +3242,7 @@
         <v>29</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>28</v>
@@ -3253,7 +3253,7 @@
         <v>30</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>7</v>
@@ -3264,7 +3264,7 @@
         <v>30</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>26</v>
@@ -3275,7 +3275,7 @@
         <v>30</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>28</v>
@@ -3286,7 +3286,7 @@
         <v>30</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>24</v>
@@ -3297,7 +3297,7 @@
         <v>31</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>5</v>
@@ -3308,7 +3308,7 @@
         <v>31</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>7</v>
@@ -3319,7 +3319,7 @@
         <v>31</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>26</v>
@@ -3330,7 +3330,7 @@
         <v>31</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>20</v>
@@ -3341,7 +3341,7 @@
         <v>31</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>30</v>
@@ -3352,7 +3352,7 @@
         <v>31</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>28</v>
@@ -3363,7 +3363,7 @@
         <v>28</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>21</v>
@@ -3374,7 +3374,7 @@
         <v>28</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>25</v>
@@ -3385,7 +3385,7 @@
         <v>28</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>5</v>
@@ -3396,7 +3396,7 @@
         <v>28</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>7</v>
@@ -3407,7 +3407,7 @@
         <v>28</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>8</v>
@@ -3418,7 +3418,7 @@
         <v>28</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>11</v>
@@ -3429,7 +3429,7 @@
         <v>28</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>20</v>
@@ -3440,7 +3440,7 @@
         <v>28</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>58</v>
@@ -3451,7 +3451,7 @@
         <v>32</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>5</v>
@@ -3462,7 +3462,7 @@
         <v>32</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>7</v>
@@ -3473,7 +3473,7 @@
         <v>32</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>33</v>
@@ -3484,7 +3484,7 @@
         <v>34</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>5</v>
@@ -3495,7 +3495,7 @@
         <v>34</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>21</v>
@@ -3506,7 +3506,7 @@
         <v>34</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>7</v>
@@ -3517,7 +3517,7 @@
         <v>34</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>28</v>
@@ -3528,7 +3528,7 @@
         <v>34</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>29</v>
@@ -3539,7 +3539,7 @@
         <v>34</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>26</v>
@@ -3550,7 +3550,7 @@
         <v>34</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>8</v>
@@ -3561,7 +3561,7 @@
         <v>34</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>9</v>
@@ -3572,7 +3572,7 @@
         <v>34</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>15</v>
@@ -3583,10 +3583,10 @@
         <v>34</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.15">
@@ -3594,7 +3594,7 @@
         <v>34</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>45</v>
@@ -3605,7 +3605,7 @@
         <v>35</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>58</v>
@@ -3616,7 +3616,7 @@
         <v>35</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>28</v>
@@ -3627,7 +3627,7 @@
         <v>35</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>28</v>
@@ -3638,7 +3638,7 @@
         <v>35</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>59</v>
@@ -3649,7 +3649,7 @@
         <v>35</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>58</v>
@@ -3660,7 +3660,7 @@
         <v>37</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>7</v>
@@ -3671,7 +3671,7 @@
         <v>37</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>9</v>
@@ -3682,7 +3682,7 @@
         <v>37</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>11</v>
@@ -3693,7 +3693,7 @@
         <v>38</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>33</v>
@@ -3704,10 +3704,10 @@
         <v>38</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.15">
@@ -3715,10 +3715,10 @@
         <v>38</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.15">
@@ -3726,7 +3726,7 @@
         <v>38</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>28</v>
@@ -3737,7 +3737,7 @@
         <v>38</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>20</v>
@@ -3748,7 +3748,7 @@
         <v>38</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>26</v>
@@ -3759,7 +3759,7 @@
         <v>38</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>39</v>
@@ -3770,7 +3770,7 @@
         <v>38</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>15</v>
@@ -3781,7 +3781,7 @@
         <v>38</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>7</v>
@@ -3792,7 +3792,7 @@
         <v>38</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>40</v>
@@ -3803,7 +3803,7 @@
         <v>41</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>5</v>
@@ -3814,7 +3814,7 @@
         <v>41</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>11</v>
@@ -3825,7 +3825,7 @@
         <v>42</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>5</v>
@@ -3836,7 +3836,7 @@
         <v>42</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>43</v>
@@ -3847,7 +3847,7 @@
         <v>44</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>45</v>
@@ -3858,7 +3858,7 @@
         <v>44</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>20</v>
@@ -3869,7 +3869,7 @@
         <v>44</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>28</v>
@@ -3880,7 +3880,7 @@
         <v>44</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>5</v>
@@ -3891,7 +3891,7 @@
         <v>46</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>5</v>
@@ -3902,7 +3902,7 @@
         <v>46</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>28</v>
@@ -3913,7 +3913,7 @@
         <v>46</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>24</v>
@@ -3924,7 +3924,7 @@
         <v>46</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>47</v>
@@ -3935,7 +3935,7 @@
         <v>46</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>28</v>
@@ -3946,7 +3946,7 @@
         <v>46</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>24</v>
@@ -3957,7 +3957,7 @@
         <v>46</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>47</v>
@@ -3968,7 +3968,7 @@
         <v>47</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>5</v>
@@ -3979,7 +3979,7 @@
         <v>47</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>7</v>
@@ -3990,7 +3990,7 @@
         <v>47</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>24</v>
@@ -4001,7 +4001,7 @@
         <v>47</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>38</v>
@@ -4012,7 +4012,7 @@
         <v>47</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>9</v>
@@ -4023,7 +4023,7 @@
         <v>47</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>28</v>
@@ -4034,7 +4034,7 @@
         <v>47</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>20</v>
@@ -4045,7 +4045,7 @@
         <v>47</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>33</v>
@@ -4056,7 +4056,7 @@
         <v>47</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>48</v>
@@ -4067,7 +4067,7 @@
         <v>40</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>5</v>
@@ -4078,7 +4078,7 @@
         <v>40</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>33</v>
@@ -4089,7 +4089,7 @@
         <v>40</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>38</v>
@@ -4100,7 +4100,7 @@
         <v>55</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>5</v>
@@ -4111,7 +4111,7 @@
         <v>55</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>15</v>
@@ -4122,10 +4122,10 @@
         <v>55</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.15">
@@ -4133,7 +4133,7 @@
         <v>55</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>45</v>
@@ -4144,10 +4144,10 @@
         <v>56</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.15">
@@ -4155,7 +4155,7 @@
         <v>56</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>58</v>
@@ -4166,10 +4166,10 @@
         <v>56</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.15">
@@ -4177,7 +4177,7 @@
         <v>56</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>59</v>
@@ -4188,10 +4188,10 @@
         <v>56</v>
       </c>
       <c r="B134" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C134" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="C134" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.15">
@@ -4199,7 +4199,7 @@
         <v>56</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>60</v>
@@ -4210,7 +4210,7 @@
         <v>57</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>17</v>
@@ -4221,7 +4221,7 @@
         <v>57</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>5</v>
@@ -4232,7 +4232,7 @@
         <v>57</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>15</v>
@@ -4240,10 +4240,10 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A139" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C139" s="1" t="s">
         <v>5</v>
@@ -4251,13 +4251,13 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A140" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.15">
@@ -4265,10 +4265,10 @@
         <v>24</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.15">
@@ -4276,10 +4276,10 @@
         <v>37</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.15">
@@ -4287,18 +4287,18 @@
         <v>38</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A144" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C144" s="2" t="s">
         <v>5</v>
@@ -4306,10 +4306,10 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A145" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C145" s="2" t="s">
         <v>21</v>
@@ -4317,10 +4317,10 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A146" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C146" s="2" t="s">
         <v>22</v>
@@ -4328,10 +4328,10 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A147" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C147" s="2" t="s">
         <v>20</v>
@@ -4339,10 +4339,10 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A148" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C148" s="2" t="s">
         <v>28</v>
@@ -4357,7 +4357,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C62C224-E054-A841-B649-DAD5203F257C}">
   <dimension ref="A1:C149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="109" workbookViewId="0">
+    <sheetView topLeftCell="A52" zoomScale="109" workbookViewId="0">
       <selection activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
@@ -4595,7 +4595,7 @@
         <v>36</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
@@ -4606,7 +4606,7 @@
         <v>36</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
@@ -5101,7 +5101,7 @@
         <v>36</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.15">
@@ -5244,7 +5244,7 @@
         <v>14</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.15">
@@ -5288,7 +5288,7 @@
         <v>36</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.15">
@@ -5365,7 +5365,7 @@
         <v>10</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.15">
@@ -5376,7 +5376,7 @@
         <v>10</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.15">
@@ -5783,7 +5783,7 @@
         <v>14</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.15">
@@ -5805,7 +5805,7 @@
         <v>14</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.15">
@@ -5827,7 +5827,7 @@
         <v>14</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.15">
@@ -5849,7 +5849,7 @@
         <v>4</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.15">
@@ -5898,7 +5898,7 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A140" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>4</v>
@@ -5909,13 +5909,13 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A141" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.15">
@@ -5926,7 +5926,7 @@
         <v>36</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.15">
@@ -5937,7 +5937,7 @@
         <v>36</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.15">
@@ -5948,12 +5948,12 @@
         <v>36</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A145" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B145" s="2" t="s">
         <v>4</v>
@@ -5964,7 +5964,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A146" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B146" s="2" t="s">
         <v>4</v>
@@ -5975,7 +5975,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A147" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B147" s="2" t="s">
         <v>10</v>
@@ -5986,7 +5986,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A148" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B148" s="2" t="s">
         <v>10</v>
@@ -5997,7 +5997,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A149" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B149" s="2" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Update edges from KBase.
</commit_message>
<xml_diff>
--- a/data/Resource Interaction Table-withIntegrated.xlsx
+++ b/data/Resource Interaction Table-withIntegrated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brooksantangelo/Documents/ReviewPaper/db_review/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8399D2C-2E5D-2D41-88E3-00920F930A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF911653-4889-BB42-9063-C313D4E0118C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10620" yWindow="760" windowWidth="21220" windowHeight="17960" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1462" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1456" uniqueCount="80">
   <si>
     <t>source</t>
   </si>
@@ -260,6 +260,9 @@
   </si>
   <si>
     <t>SNOMEDCT_Disease</t>
+  </si>
+  <si>
+    <t>KEGG Pathways</t>
   </si>
 </sst>
 </file>
@@ -530,10 +533,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D149"/>
+  <dimension ref="A1:D148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="E130" sqref="E130"/>
+    <sheetView topLeftCell="A98" zoomScale="142" workbookViewId="0">
+      <selection activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1739,7 +1742,7 @@
         <v>75</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1749,8 +1752,8 @@
       <c r="B110" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C110" s="1" t="s">
-        <v>24</v>
+      <c r="C110" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1758,21 +1761,21 @@
         <v>46</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A112" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B112" s="1" t="s">
+      <c r="B112" s="2" t="s">
         <v>75</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1782,19 +1785,19 @@
       <c r="B113" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C113" s="1" t="s">
-        <v>24</v>
+      <c r="C113" s="2" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A114" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1805,7 +1808,7 @@
         <v>74</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1813,10 +1816,10 @@
         <v>47</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1827,7 +1830,7 @@
         <v>75</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1838,7 +1841,7 @@
         <v>75</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1849,7 +1852,7 @@
         <v>75</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1860,7 +1863,7 @@
         <v>75</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1868,10 +1871,10 @@
         <v>47</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1879,21 +1882,21 @@
         <v>47</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="13" x14ac:dyDescent="0.15">
       <c r="A123" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1904,29 +1907,29 @@
         <v>74</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A125" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A126" s="1" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1937,7 +1940,7 @@
         <v>74</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1945,10 +1948,10 @@
         <v>55</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1959,18 +1962,18 @@
         <v>75</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A130" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1981,7 +1984,7 @@
         <v>75</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1992,7 +1995,7 @@
         <v>75</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2003,7 +2006,7 @@
         <v>75</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2014,7 +2017,7 @@
         <v>75</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2025,18 +2028,18 @@
         <v>75</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A136" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>60</v>
+        <v>17</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2047,7 +2050,7 @@
         <v>75</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2055,21 +2058,21 @@
         <v>57</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="139" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A139" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2077,26 +2080,26 @@
         <v>62</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A141" s="1" t="s">
-        <v>62</v>
+      <c r="A141" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C141" s="1" t="s">
-        <v>63</v>
+      <c r="C141" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A142" s="2" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>74</v>
@@ -2107,7 +2110,7 @@
     </row>
     <row r="143" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A143" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>74</v>
@@ -2118,13 +2121,13 @@
     </row>
     <row r="144" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A144" s="2" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>74</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>64</v>
+        <v>5</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2132,10 +2135,10 @@
         <v>68</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2146,7 +2149,7 @@
         <v>75</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="147" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2157,28 +2160,17 @@
         <v>75</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="148" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A148" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A149" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B149" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C149" s="2" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2196,7 +2188,7 @@
   <dimension ref="A1:B62"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4355,10 +4347,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C62C224-E054-A841-B649-DAD5203F257C}">
-  <dimension ref="A1:C149"/>
+  <dimension ref="A1:C148"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScale="109" workbookViewId="0">
-      <selection activeCell="E75" sqref="E75"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="109" workbookViewId="0">
+      <selection activeCell="F117" sqref="F117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5560,10 +5552,10 @@
         <v>46</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.15">
@@ -5571,10 +5563,10 @@
         <v>46</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.15">
@@ -5582,10 +5574,10 @@
         <v>46</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.15">
@@ -5596,7 +5588,7 @@
         <v>10</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.15">
@@ -5604,21 +5596,21 @@
         <v>46</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>24</v>
+        <v>79</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A114" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.15">
@@ -5626,10 +5618,10 @@
         <v>47</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.15">
@@ -5640,7 +5632,7 @@
         <v>6</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.15">
@@ -5651,7 +5643,7 @@
         <v>6</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.15">
@@ -5662,7 +5654,7 @@
         <v>6</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.15">
@@ -5673,7 +5665,7 @@
         <v>6</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.15">
@@ -5681,10 +5673,10 @@
         <v>47</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.15">
@@ -5695,7 +5687,7 @@
         <v>10</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.15">
@@ -5706,18 +5698,18 @@
         <v>10</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A123" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.15">
@@ -5725,10 +5717,10 @@
         <v>40</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.15">
@@ -5739,18 +5731,18 @@
         <v>10</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A126" s="1" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.15">
@@ -5758,10 +5750,10 @@
         <v>55</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.15">
@@ -5772,7 +5764,7 @@
         <v>14</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.15">
@@ -5783,18 +5775,18 @@
         <v>14</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A130" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.15">
@@ -5805,7 +5797,7 @@
         <v>14</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.15">
@@ -5816,7 +5808,7 @@
         <v>14</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.15">
@@ -5824,10 +5816,10 @@
         <v>56</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.15">
@@ -5838,7 +5830,7 @@
         <v>4</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.15">
@@ -5849,18 +5841,18 @@
         <v>4</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A136" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>60</v>
+        <v>17</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.15">
@@ -5871,7 +5863,7 @@
         <v>4</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.15">
@@ -5879,21 +5871,21 @@
         <v>57</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A139" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.15">
@@ -5901,26 +5893,26 @@
         <v>62</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A141" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B141" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C141" s="1" t="s">
-        <v>63</v>
+      <c r="A141" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A142" s="2" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="B142" s="2" t="s">
         <v>36</v>
@@ -5931,7 +5923,7 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A143" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B143" s="2" t="s">
         <v>36</v>
@@ -5942,13 +5934,13 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A144" s="2" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>64</v>
+        <v>5</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.15">
@@ -5959,7 +5951,7 @@
         <v>4</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.15">
@@ -5967,10 +5959,10 @@
         <v>68</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.15">
@@ -5981,28 +5973,17 @@
         <v>10</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A148" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A149" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B149" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C149" s="2" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove EFO not a disease db.
</commit_message>
<xml_diff>
--- a/data/Resource Interaction Table-withIntegrated.xlsx
+++ b/data/Resource Interaction Table-withIntegrated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brooksantangelo/Documents/ReviewPaper/db_review/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D2FA0AD-6D70-514A-AAB2-90C0CB75D35A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6156FD21-4D46-514E-B7DC-7BC037FDDE69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10620" yWindow="760" windowWidth="21220" windowHeight="17960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10620" yWindow="760" windowWidth="21220" windowHeight="17960" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1445" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="78">
   <si>
     <t>source</t>
   </si>
@@ -209,9 +209,6 @@
   </si>
   <si>
     <t>BugSigDB</t>
-  </si>
-  <si>
-    <t>EFO</t>
   </si>
   <si>
     <t>PO</t>
@@ -530,10 +527,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D147"/>
+  <dimension ref="A1:D146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="142" workbookViewId="0">
-      <selection activeCell="D92" sqref="D92"/>
+    <sheetView topLeftCell="A121" zoomScale="142" workbookViewId="0">
+      <selection activeCell="A139" sqref="A139:XFD139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -558,7 +555,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
@@ -569,7 +566,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -580,7 +577,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>8</v>
@@ -591,7 +588,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>9</v>
@@ -602,7 +599,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>11</v>
@@ -613,7 +610,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>5</v>
@@ -624,7 +621,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>13</v>
@@ -635,7 +632,7 @@
         <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>15</v>
@@ -646,7 +643,7 @@
         <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>5</v>
@@ -657,7 +654,7 @@
         <v>16</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>17</v>
@@ -668,7 +665,7 @@
         <v>16</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>18</v>
@@ -679,7 +676,7 @@
         <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>13</v>
@@ -690,7 +687,7 @@
         <v>19</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>20</v>
@@ -701,7 +698,7 @@
         <v>9</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>21</v>
@@ -712,7 +709,7 @@
         <v>9</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>7</v>
@@ -723,7 +720,7 @@
         <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>8</v>
@@ -734,7 +731,7 @@
         <v>9</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>20</v>
@@ -745,7 +742,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>22</v>
@@ -756,7 +753,7 @@
         <v>9</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>23</v>
@@ -767,10 +764,10 @@
         <v>9</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -778,10 +775,10 @@
         <v>9</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -789,7 +786,7 @@
         <v>24</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>25</v>
@@ -800,7 +797,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>7</v>
@@ -811,7 +808,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>8</v>
@@ -822,7 +819,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>26</v>
@@ -833,7 +830,7 @@
         <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>11</v>
@@ -844,7 +841,7 @@
         <v>24</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>20</v>
@@ -855,7 +852,7 @@
         <v>24</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>22</v>
@@ -866,7 +863,7 @@
         <v>24</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>9</v>
@@ -877,7 +874,7 @@
         <v>27</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>7</v>
@@ -888,7 +885,7 @@
         <v>27</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>8</v>
@@ -899,7 +896,7 @@
         <v>27</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>26</v>
@@ -910,7 +907,7 @@
         <v>27</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>20</v>
@@ -921,7 +918,7 @@
         <v>27</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>9</v>
@@ -932,7 +929,7 @@
         <v>27</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>24</v>
@@ -943,7 +940,7 @@
         <v>27</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>28</v>
@@ -954,7 +951,7 @@
         <v>29</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>7</v>
@@ -965,7 +962,7 @@
         <v>29</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>8</v>
@@ -976,7 +973,7 @@
         <v>29</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>13</v>
@@ -987,7 +984,7 @@
         <v>29</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>26</v>
@@ -998,7 +995,7 @@
         <v>29</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>11</v>
@@ -1009,7 +1006,7 @@
         <v>29</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>20</v>
@@ -1020,7 +1017,7 @@
         <v>29</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>23</v>
@@ -1031,7 +1028,7 @@
         <v>29</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>24</v>
@@ -1042,7 +1039,7 @@
         <v>29</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>30</v>
@@ -1053,7 +1050,7 @@
         <v>29</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>9</v>
@@ -1064,7 +1061,7 @@
         <v>29</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>28</v>
@@ -1075,7 +1072,7 @@
         <v>30</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>7</v>
@@ -1086,7 +1083,7 @@
         <v>30</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>26</v>
@@ -1097,7 +1094,7 @@
         <v>30</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>28</v>
@@ -1108,7 +1105,7 @@
         <v>30</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>24</v>
@@ -1119,7 +1116,7 @@
         <v>31</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>5</v>
@@ -1130,7 +1127,7 @@
         <v>31</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>7</v>
@@ -1141,7 +1138,7 @@
         <v>31</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>26</v>
@@ -1152,7 +1149,7 @@
         <v>31</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>20</v>
@@ -1163,7 +1160,7 @@
         <v>31</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>30</v>
@@ -1174,7 +1171,7 @@
         <v>31</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>28</v>
@@ -1185,7 +1182,7 @@
         <v>28</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>21</v>
@@ -1196,7 +1193,7 @@
         <v>28</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>25</v>
@@ -1207,7 +1204,7 @@
         <v>28</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>5</v>
@@ -1218,7 +1215,7 @@
         <v>28</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>7</v>
@@ -1229,7 +1226,7 @@
         <v>28</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>8</v>
@@ -1240,7 +1237,7 @@
         <v>28</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>11</v>
@@ -1251,7 +1248,7 @@
         <v>28</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>20</v>
@@ -1262,7 +1259,7 @@
         <v>28</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>57</v>
@@ -1273,10 +1270,10 @@
         <v>28</v>
       </c>
       <c r="B67" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1284,7 +1281,7 @@
         <v>32</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>5</v>
@@ -1295,7 +1292,7 @@
         <v>32</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>7</v>
@@ -1306,7 +1303,7 @@
         <v>32</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>33</v>
@@ -1317,7 +1314,7 @@
         <v>34</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>5</v>
@@ -1328,7 +1325,7 @@
         <v>34</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>21</v>
@@ -1339,7 +1336,7 @@
         <v>34</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>7</v>
@@ -1350,7 +1347,7 @@
         <v>34</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>28</v>
@@ -1361,7 +1358,7 @@
         <v>34</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>29</v>
@@ -1372,7 +1369,7 @@
         <v>34</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>26</v>
@@ -1383,7 +1380,7 @@
         <v>34</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>8</v>
@@ -1394,7 +1391,7 @@
         <v>34</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>9</v>
@@ -1405,7 +1402,7 @@
         <v>34</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>15</v>
@@ -1416,10 +1413,10 @@
         <v>34</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -1427,7 +1424,7 @@
         <v>34</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>44</v>
@@ -1438,7 +1435,7 @@
         <v>35</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>57</v>
@@ -1450,7 +1447,7 @@
         <v>35</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>28</v>
@@ -1461,10 +1458,10 @@
         <v>35</v>
       </c>
       <c r="B84" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C84" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -1472,7 +1469,7 @@
         <v>35</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>58</v>
@@ -1483,7 +1480,7 @@
         <v>35</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>57</v>
@@ -1494,7 +1491,7 @@
         <v>37</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>7</v>
@@ -1505,7 +1502,7 @@
         <v>37</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>9</v>
@@ -1516,7 +1513,7 @@
         <v>37</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>11</v>
@@ -1527,7 +1524,7 @@
         <v>38</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>33</v>
@@ -1538,10 +1535,10 @@
         <v>38</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -1549,10 +1546,10 @@
         <v>38</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -1560,7 +1557,7 @@
         <v>38</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>28</v>
@@ -1571,7 +1568,7 @@
         <v>38</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>20</v>
@@ -1582,7 +1579,7 @@
         <v>38</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>26</v>
@@ -1593,7 +1590,7 @@
         <v>38</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>15</v>
@@ -1604,7 +1601,7 @@
         <v>38</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>7</v>
@@ -1615,7 +1612,7 @@
         <v>38</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>39</v>
@@ -1626,7 +1623,7 @@
         <v>40</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>5</v>
@@ -1637,7 +1634,7 @@
         <v>40</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>11</v>
@@ -1648,7 +1645,7 @@
         <v>41</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>5</v>
@@ -1659,7 +1656,7 @@
         <v>41</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>42</v>
@@ -1670,7 +1667,7 @@
         <v>43</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>44</v>
@@ -1681,7 +1678,7 @@
         <v>43</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>20</v>
@@ -1692,7 +1689,7 @@
         <v>43</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>28</v>
@@ -1703,7 +1700,7 @@
         <v>43</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>5</v>
@@ -1714,7 +1711,7 @@
         <v>45</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>5</v>
@@ -1725,7 +1722,7 @@
         <v>45</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>25</v>
@@ -1736,7 +1733,7 @@
         <v>45</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C109" s="2" t="s">
         <v>22</v>
@@ -1747,7 +1744,7 @@
         <v>45</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>33</v>
@@ -1758,7 +1755,7 @@
         <v>45</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>20</v>
@@ -1769,10 +1766,10 @@
         <v>45</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="13" x14ac:dyDescent="0.15">
@@ -1780,7 +1777,7 @@
         <v>46</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>5</v>
@@ -1791,7 +1788,7 @@
         <v>46</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>7</v>
@@ -1802,7 +1799,7 @@
         <v>46</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>24</v>
@@ -1813,7 +1810,7 @@
         <v>46</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>38</v>
@@ -1824,7 +1821,7 @@
         <v>46</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>9</v>
@@ -1835,7 +1832,7 @@
         <v>46</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>28</v>
@@ -1846,7 +1843,7 @@
         <v>46</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>20</v>
@@ -1857,7 +1854,7 @@
         <v>46</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>33</v>
@@ -1868,7 +1865,7 @@
         <v>46</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>47</v>
@@ -1879,7 +1876,7 @@
         <v>39</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>5</v>
@@ -1890,7 +1887,7 @@
         <v>39</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>33</v>
@@ -1901,7 +1898,7 @@
         <v>39</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>38</v>
@@ -1912,7 +1909,7 @@
         <v>54</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>5</v>
@@ -1923,7 +1920,7 @@
         <v>54</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>15</v>
@@ -1934,7 +1931,7 @@
         <v>54</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>60</v>
@@ -1945,7 +1942,7 @@
         <v>54</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>44</v>
@@ -1956,10 +1953,10 @@
         <v>55</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1967,7 +1964,7 @@
         <v>55</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>57</v>
@@ -1978,7 +1975,7 @@
         <v>55</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>60</v>
@@ -1989,7 +1986,7 @@
         <v>55</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>58</v>
@@ -2000,10 +1997,10 @@
         <v>55</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2011,7 +2008,7 @@
         <v>55</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>59</v>
@@ -2022,7 +2019,7 @@
         <v>56</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>17</v>
@@ -2033,7 +2030,7 @@
         <v>56</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>5</v>
@@ -2044,7 +2041,7 @@
         <v>56</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>15</v>
@@ -2055,108 +2052,97 @@
         <v>61</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="139" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A139" s="1" t="s">
-        <v>61</v>
+      <c r="A139" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C139" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C139" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A140" s="2" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A141" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A142" s="2" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>63</v>
+        <v>5</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A143" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A144" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A145" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A146" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A147" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B147" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C147" s="2" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2171,10 +2157,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B61"/>
+  <dimension ref="A1:B60"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:XFD39"/>
+      <selection activeCell="A53" sqref="A53:XFD53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2316,7 +2302,7 @@
         <v>28</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2324,7 +2310,7 @@
         <v>24</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2332,7 +2318,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2340,7 +2326,7 @@
         <v>30</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2348,7 +2334,7 @@
         <v>29</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2372,7 +2358,7 @@
         <v>46</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2380,7 +2366,7 @@
         <v>38</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2396,7 +2382,7 @@
         <v>3</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2404,7 +2390,7 @@
         <v>12</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2412,7 +2398,7 @@
         <v>16</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2420,7 +2406,7 @@
         <v>19</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2428,7 +2414,7 @@
         <v>27</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2436,7 +2422,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2444,7 +2430,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2452,7 +2438,7 @@
         <v>34</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2460,7 +2446,7 @@
         <v>35</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2468,7 +2454,7 @@
         <v>37</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2476,7 +2462,7 @@
         <v>40</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2484,7 +2470,7 @@
         <v>41</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2492,7 +2478,7 @@
         <v>39</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2500,7 +2486,7 @@
         <v>43</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2508,7 +2494,7 @@
         <v>45</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2516,7 +2502,7 @@
         <v>54</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2524,7 +2510,7 @@
         <v>55</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2532,7 +2518,7 @@
         <v>56</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2545,7 +2531,7 @@
     </row>
     <row r="46" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>53</v>
@@ -2569,7 +2555,7 @@
     </row>
     <row r="49" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>50</v>
@@ -2588,87 +2574,79 @@
         <v>61</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B52" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A53" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A54" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A55" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A56" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A57" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A58" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A57" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="2" t="s">
+      <c r="B58" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A59" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A60" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -2678,10 +2656,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C62B794-0898-E64A-A668-9B45516A9588}">
-  <dimension ref="A1:C147"/>
+  <dimension ref="A1:C146"/>
   <sheetViews>
-    <sheetView topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="A95" sqref="A95:XFD95"/>
+    <sheetView topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="E155" sqref="E155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2706,7 +2684,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
@@ -2717,7 +2695,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -2728,7 +2706,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>8</v>
@@ -2739,7 +2717,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>9</v>
@@ -2750,7 +2728,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>11</v>
@@ -2761,7 +2739,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>5</v>
@@ -2772,7 +2750,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>13</v>
@@ -2783,7 +2761,7 @@
         <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>15</v>
@@ -2794,7 +2772,7 @@
         <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>5</v>
@@ -2805,7 +2783,7 @@
         <v>16</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>17</v>
@@ -2816,7 +2794,7 @@
         <v>16</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>18</v>
@@ -2827,7 +2805,7 @@
         <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>13</v>
@@ -2838,7 +2816,7 @@
         <v>19</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>20</v>
@@ -2849,7 +2827,7 @@
         <v>9</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>21</v>
@@ -2860,7 +2838,7 @@
         <v>9</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>7</v>
@@ -2871,7 +2849,7 @@
         <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>8</v>
@@ -2882,7 +2860,7 @@
         <v>9</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>20</v>
@@ -2893,7 +2871,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>22</v>
@@ -2904,7 +2882,7 @@
         <v>9</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>23</v>
@@ -2915,10 +2893,10 @@
         <v>9</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
@@ -2926,10 +2904,10 @@
         <v>9</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
@@ -2937,7 +2915,7 @@
         <v>24</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>25</v>
@@ -2948,7 +2926,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>7</v>
@@ -2959,7 +2937,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>8</v>
@@ -2970,7 +2948,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>26</v>
@@ -2981,7 +2959,7 @@
         <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>11</v>
@@ -2992,7 +2970,7 @@
         <v>24</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>20</v>
@@ -3003,7 +2981,7 @@
         <v>24</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>22</v>
@@ -3014,7 +2992,7 @@
         <v>24</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>9</v>
@@ -3025,7 +3003,7 @@
         <v>27</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>7</v>
@@ -3036,7 +3014,7 @@
         <v>27</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>8</v>
@@ -3047,7 +3025,7 @@
         <v>27</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>26</v>
@@ -3058,7 +3036,7 @@
         <v>27</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>20</v>
@@ -3069,7 +3047,7 @@
         <v>27</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>9</v>
@@ -3080,7 +3058,7 @@
         <v>27</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>24</v>
@@ -3091,7 +3069,7 @@
         <v>27</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>28</v>
@@ -3102,7 +3080,7 @@
         <v>29</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>7</v>
@@ -3113,7 +3091,7 @@
         <v>29</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>8</v>
@@ -3124,7 +3102,7 @@
         <v>29</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>13</v>
@@ -3135,7 +3113,7 @@
         <v>29</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>26</v>
@@ -3146,7 +3124,7 @@
         <v>29</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>11</v>
@@ -3157,7 +3135,7 @@
         <v>29</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>20</v>
@@ -3168,7 +3146,7 @@
         <v>29</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>23</v>
@@ -3179,7 +3157,7 @@
         <v>29</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>24</v>
@@ -3190,7 +3168,7 @@
         <v>29</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>30</v>
@@ -3201,7 +3179,7 @@
         <v>29</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>9</v>
@@ -3212,7 +3190,7 @@
         <v>29</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>28</v>
@@ -3223,7 +3201,7 @@
         <v>30</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>7</v>
@@ -3234,7 +3212,7 @@
         <v>30</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>26</v>
@@ -3245,7 +3223,7 @@
         <v>30</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>28</v>
@@ -3256,7 +3234,7 @@
         <v>30</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>24</v>
@@ -3267,7 +3245,7 @@
         <v>31</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>5</v>
@@ -3278,7 +3256,7 @@
         <v>31</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>7</v>
@@ -3289,7 +3267,7 @@
         <v>31</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>26</v>
@@ -3300,7 +3278,7 @@
         <v>31</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>20</v>
@@ -3311,7 +3289,7 @@
         <v>31</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>30</v>
@@ -3322,7 +3300,7 @@
         <v>31</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>28</v>
@@ -3333,7 +3311,7 @@
         <v>28</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>21</v>
@@ -3344,7 +3322,7 @@
         <v>28</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>25</v>
@@ -3355,7 +3333,7 @@
         <v>28</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>5</v>
@@ -3366,7 +3344,7 @@
         <v>28</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>7</v>
@@ -3377,7 +3355,7 @@
         <v>28</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>8</v>
@@ -3388,7 +3366,7 @@
         <v>28</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>11</v>
@@ -3399,7 +3377,7 @@
         <v>28</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>20</v>
@@ -3410,7 +3388,7 @@
         <v>28</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>57</v>
@@ -3421,7 +3399,7 @@
         <v>32</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>5</v>
@@ -3432,7 +3410,7 @@
         <v>32</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>7</v>
@@ -3443,7 +3421,7 @@
         <v>32</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>33</v>
@@ -3454,7 +3432,7 @@
         <v>34</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>5</v>
@@ -3465,7 +3443,7 @@
         <v>34</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>21</v>
@@ -3476,7 +3454,7 @@
         <v>34</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>7</v>
@@ -3487,7 +3465,7 @@
         <v>34</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>28</v>
@@ -3498,7 +3476,7 @@
         <v>34</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>29</v>
@@ -3509,7 +3487,7 @@
         <v>34</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>26</v>
@@ -3520,7 +3498,7 @@
         <v>34</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>8</v>
@@ -3531,7 +3509,7 @@
         <v>34</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>9</v>
@@ -3542,7 +3520,7 @@
         <v>34</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>15</v>
@@ -3553,10 +3531,10 @@
         <v>34</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.15">
@@ -3564,7 +3542,7 @@
         <v>34</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>44</v>
@@ -3575,7 +3553,7 @@
         <v>35</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>57</v>
@@ -3586,7 +3564,7 @@
         <v>35</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>28</v>
@@ -3597,7 +3575,7 @@
         <v>35</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>28</v>
@@ -3608,7 +3586,7 @@
         <v>35</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>58</v>
@@ -3619,7 +3597,7 @@
         <v>35</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>57</v>
@@ -3630,7 +3608,7 @@
         <v>37</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>7</v>
@@ -3641,7 +3619,7 @@
         <v>37</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>9</v>
@@ -3652,7 +3630,7 @@
         <v>37</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>11</v>
@@ -3663,7 +3641,7 @@
         <v>38</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>33</v>
@@ -3674,10 +3652,10 @@
         <v>38</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.15">
@@ -3685,10 +3663,10 @@
         <v>38</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.15">
@@ -3696,7 +3674,7 @@
         <v>38</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>28</v>
@@ -3707,7 +3685,7 @@
         <v>38</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>20</v>
@@ -3718,7 +3696,7 @@
         <v>38</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>26</v>
@@ -3729,7 +3707,7 @@
         <v>38</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>15</v>
@@ -3740,7 +3718,7 @@
         <v>38</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>7</v>
@@ -3751,7 +3729,7 @@
         <v>38</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>39</v>
@@ -3762,7 +3740,7 @@
         <v>40</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>5</v>
@@ -3773,7 +3751,7 @@
         <v>40</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>11</v>
@@ -3784,7 +3762,7 @@
         <v>41</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>5</v>
@@ -3795,7 +3773,7 @@
         <v>41</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>42</v>
@@ -3806,7 +3784,7 @@
         <v>43</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>44</v>
@@ -3817,7 +3795,7 @@
         <v>43</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>20</v>
@@ -3828,7 +3806,7 @@
         <v>43</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>28</v>
@@ -3839,7 +3817,7 @@
         <v>43</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>5</v>
@@ -3850,7 +3828,7 @@
         <v>45</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>5</v>
@@ -3861,7 +3839,7 @@
         <v>45</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>28</v>
@@ -3872,7 +3850,7 @@
         <v>45</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>24</v>
@@ -3883,7 +3861,7 @@
         <v>45</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>46</v>
@@ -3894,7 +3872,7 @@
         <v>45</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>28</v>
@@ -3905,7 +3883,7 @@
         <v>45</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>24</v>
@@ -3916,7 +3894,7 @@
         <v>45</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>46</v>
@@ -3927,7 +3905,7 @@
         <v>46</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>5</v>
@@ -3938,7 +3916,7 @@
         <v>46</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>7</v>
@@ -3949,7 +3927,7 @@
         <v>46</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>24</v>
@@ -3960,7 +3938,7 @@
         <v>46</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>38</v>
@@ -3971,7 +3949,7 @@
         <v>46</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>9</v>
@@ -3982,7 +3960,7 @@
         <v>46</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>28</v>
@@ -3993,7 +3971,7 @@
         <v>46</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>20</v>
@@ -4004,7 +3982,7 @@
         <v>46</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>33</v>
@@ -4015,7 +3993,7 @@
         <v>46</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>47</v>
@@ -4026,7 +4004,7 @@
         <v>39</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>5</v>
@@ -4037,7 +4015,7 @@
         <v>39</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>33</v>
@@ -4048,7 +4026,7 @@
         <v>39</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>38</v>
@@ -4059,7 +4037,7 @@
         <v>54</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>5</v>
@@ -4070,7 +4048,7 @@
         <v>54</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>15</v>
@@ -4081,7 +4059,7 @@
         <v>54</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>60</v>
@@ -4092,7 +4070,7 @@
         <v>54</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>44</v>
@@ -4103,10 +4081,10 @@
         <v>55</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.15">
@@ -4114,7 +4092,7 @@
         <v>55</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>57</v>
@@ -4125,7 +4103,7 @@
         <v>55</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>60</v>
@@ -4136,7 +4114,7 @@
         <v>55</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>58</v>
@@ -4147,10 +4125,10 @@
         <v>55</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.15">
@@ -4158,7 +4136,7 @@
         <v>55</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>59</v>
@@ -4169,7 +4147,7 @@
         <v>56</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>17</v>
@@ -4180,7 +4158,7 @@
         <v>56</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>5</v>
@@ -4191,7 +4169,7 @@
         <v>56</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>15</v>
@@ -4202,108 +4180,97 @@
         <v>61</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A139" s="1" t="s">
-        <v>61</v>
+      <c r="A139" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C139" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C139" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A140" s="2" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A141" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A142" s="2" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>63</v>
+        <v>5</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A143" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A144" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A145" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A146" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A147" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B147" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C147" s="2" t="s">
         <v>28</v>
       </c>
     </row>
@@ -4314,10 +4281,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C62C224-E054-A841-B649-DAD5203F257C}">
-  <dimension ref="A1:C147"/>
+  <dimension ref="A1:C146"/>
   <sheetViews>
-    <sheetView topLeftCell="A95" zoomScale="109" workbookViewId="0">
-      <selection activeCell="F111" sqref="F111"/>
+    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="109" workbookViewId="0">
+      <selection activeCell="F144" sqref="F144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4554,7 +4521,7 @@
         <v>36</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
@@ -4565,7 +4532,7 @@
         <v>36</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
@@ -5060,7 +5027,7 @@
         <v>36</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.15">
@@ -5203,7 +5170,7 @@
         <v>14</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.15">
@@ -5247,7 +5214,7 @@
         <v>36</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.15">
@@ -5324,7 +5291,7 @@
         <v>10</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.15">
@@ -5335,7 +5302,7 @@
         <v>10</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.15">
@@ -5555,7 +5522,7 @@
         <v>36</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.15">
@@ -5742,7 +5709,7 @@
         <v>14</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.15">
@@ -5786,7 +5753,7 @@
         <v>4</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.15">
@@ -5845,101 +5812,90 @@
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A139" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B139" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C139" s="1" t="s">
+      <c r="A139" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C139" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A140" s="2" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="B140" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A141" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B141" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A142" s="2" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>63</v>
+        <v>5</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A143" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B143" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A144" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A145" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B145" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A146" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A147" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B147" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C147" s="2" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>